<commit_message>
Add user sheet management features and update various components
</commit_message>
<xml_diff>
--- a/data/raw/건물토지매매.xlsx
+++ b/data/raw/건물토지매매.xlsx
@@ -10695,7 +10695,7 @@
       </c>
       <c r="P107" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="Q107" t="inlineStr">
@@ -10781,7 +10781,7 @@
       </c>
       <c r="P108" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="Q108" t="inlineStr">

</xml_diff>